<commit_message>
Amended some of the formulas in stage 2 to expand the keyword match to 30.
I also lowered the threhold to 10% appearance.  
Maybe try lowering this to 5%.
</commit_message>
<xml_diff>
--- a/Results_ML_Models/Decision Tree Results for_Nograms.xlsx
+++ b/Results_ML_Models/Decision Tree Results for_Nograms.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Accuracy_train</t>
   </si>
@@ -22,31 +22,13 @@
     <t>Accuracy_test</t>
   </si>
   <si>
+    <t>DocketSheet_WordMatches_TopWords_Nograms_CalculationIII_Correlation_Coefficient_Top15_highest_COCOEF.xlsx.xlsx</t>
+  </si>
+  <si>
     <t>DocketSheet_WordMatches_TopWords_Nograms_CalculationII_AVG_not_zero_Top15_highest_STDV.xlsx.xlsx</t>
   </si>
   <si>
-    <t>DocketSheet_WordMatches_TopWords_Nograms_CalculationII_AVG_not_zero_Top5_highest_STDV_AVG_below_20prct.xlsx.xlsx</t>
-  </si>
-  <si>
-    <t>DocketSheet_WordMatches_TopWords_Nograms_CalculationI_homebrew_STDV_Top5_highest_STDV_lowest_AVG.xlsx.xlsx</t>
-  </si>
-  <si>
-    <t>DocketSheet_WordMatches_TopWords_Nograms_CalculationIII_Correlation_Coefficient_Top15_highest_COCOEF.xlsx.xlsx</t>
-  </si>
-  <si>
-    <t>DocketSheet_WordMatches_TopWords_Nograms_CalculationI_homebrew_STDV_Top5_highest_STDV_AVG_below_20prct.xlsx.xlsx</t>
-  </si>
-  <si>
-    <t>DocketSheet_WordMatches_TopWords_Nograms_CalculationII_AVG_not_zero_Top5_lowest_STDV_highest_AVG.xlsx.xlsx</t>
-  </si>
-  <si>
-    <t>DocketSheet_WordMatches_TopWords_Nograms_CalculationI_homebrew_STDV_Top5_lowest_STDV_highest_AVG.xlsx.xlsx</t>
-  </si>
-  <si>
-    <t>DocketSheet_WordMatches_TopWords_Nograms_CalculationII_AVG_not_zero_Top5_highest_STDV_lowest_AVG.xlsx.xlsx</t>
-  </si>
-  <si>
-    <t>DocketSheet_WordMatches_TopWords_Nograms_CalculationIII_Correlation_Coefficient_Top5_lowest_COCOEF_highest_AVG.xlsx.xlsx</t>
+    <t>DocketSheet_WordMatches_TopWords_Nograms_CalculationI_homebrew_STDV_Top15_highest_STDV.xlsx.xlsx</t>
   </si>
 </sst>
 </file>
@@ -404,7 +386,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -423,10 +405,10 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>0.96</v>
+        <v>0.97</v>
       </c>
       <c r="C2">
-        <v>0.84</v>
+        <v>0.86</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -434,10 +416,10 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>0.87</v>
+        <v>0.96</v>
       </c>
       <c r="C3">
-        <v>0.8100000000000001</v>
+        <v>0.85</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -445,76 +427,10 @@
         <v>4</v>
       </c>
       <c r="B4">
-        <v>0.82</v>
+        <v>0.96</v>
       </c>
       <c r="C4">
-        <v>0.78</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5">
-        <v>0.87</v>
-      </c>
-      <c r="C5">
-        <v>0.76</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6">
-        <v>0.87</v>
-      </c>
-      <c r="C6">
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7">
-        <v>0.74</v>
-      </c>
-      <c r="C7">
-        <v>0.6899999999999999</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8">
-        <v>0.7</v>
-      </c>
-      <c r="C8">
-        <v>0.66</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9">
-        <v>0.73</v>
-      </c>
-      <c r="C9">
-        <v>0.64</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10">
-        <v>0.67</v>
-      </c>
-      <c r="C10">
-        <v>0.6</v>
+        <v>0.84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>